<commit_message>
fix displaying combi found
</commit_message>
<xml_diff>
--- a/stl/digit_position.xlsx
+++ b/stl/digit_position.xlsx
@@ -47,52 +47,52 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00720763"/>
+        <fgColor rgb="00747156"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00720949"/>
+        <fgColor rgb="00742068"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00699951"/>
+        <fgColor rgb="00765346"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00730568"/>
+        <fgColor rgb="00773545"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00750323"/>
+        <fgColor rgb="00746318"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00716431"/>
+        <fgColor rgb="00737622"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00754229"/>
+        <fgColor rgb="00721267"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00755844"/>
+        <fgColor rgb="00753525"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00737611"/>
+        <fgColor rgb="00699607"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00748852"/>
+        <fgColor rgb="00745133"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>

<commit_message>
implement cfscrape and fake_useragent libraries, add more http request headers
</commit_message>
<xml_diff>
--- a/stl/digit_position.xlsx
+++ b/stl/digit_position.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -47,52 +47,52 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00754560"/>
+        <fgColor rgb="00712727"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00698798"/>
+        <fgColor rgb="00717286"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00702637"/>
+        <fgColor rgb="00701894"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00773821"/>
+        <fgColor rgb="00709774"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00732036"/>
+        <fgColor rgb="00741598"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00739750"/>
+        <fgColor rgb="00771965"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00708869"/>
+        <fgColor rgb="00767261"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00739767"/>
+        <fgColor rgb="00749453"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00778199"/>
+        <fgColor rgb="00775637"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00741589"/>
+        <fgColor rgb="00707024"/>
       </patternFill>
     </fill>
   </fills>

</xml_diff>